<commit_message>
updated after 2nd race
</commit_message>
<xml_diff>
--- a/processor/config2019.xlsx
+++ b/processor/config2019.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Data\Problems\vkct\processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890C5B7B-1805-49A2-9A16-488D4BE9E87D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D88297-1230-4885-A707-36BCC4D806AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15090" activeTab="2" xr2:uid="{15338A40-4FCA-4B48-85DC-9A39AA2E7524}"/>
+    <workbookView xWindow="3780" yWindow="3810" windowWidth="21600" windowHeight="12300" xr2:uid="{15338A40-4FCA-4B48-85DC-9A39AA2E7524}"/>
   </bookViews>
   <sheets>
     <sheet name="Kategorie" sheetId="1" r:id="rId1"/>
     <sheet name="M1" sheetId="2" r:id="rId2"/>
     <sheet name="M2" sheetId="3" r:id="rId3"/>
+    <sheet name="Ml. Žáci" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Kategorie">Kategorie!$A$4:$E$23</definedName>
+    <definedName name="Kategorie">Kategorie!$A$4:$E$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
   <si>
     <t>Rok:</t>
   </si>
@@ -125,6 +126,27 @@
   </si>
   <si>
     <t>..\2019-src\zavod5\Kasava2019.xlsx</t>
+  </si>
+  <si>
+    <t>..\2019-src\zavod1\HradniOkruh2019-b.xlsx</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>alternativní</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Ml. Žáci</t>
   </si>
 </sst>
 </file>
@@ -500,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F60167-74EE-4847-B777-F54D2D3F9AAF}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,31 +599,46 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4">
+        <f>$B$1-C6</f>
+        <v>2007</v>
+      </c>
+      <c r="E6" s="4">
+        <f>$B$1-B6</f>
+        <v>2008</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>50</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>100</v>
       </c>
-      <c r="D7" s="4">
-        <f>$B$1-C7</f>
+      <c r="D8" s="4">
+        <f>$B$1-C8</f>
         <v>1919</v>
       </c>
-      <c r="E7" s="4">
-        <f>$B$1-B7</f>
+      <c r="E8" s="4">
+        <f>$B$1-B8</f>
         <v>1969</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
@@ -666,6 +703,10 @@
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -675,10 +716,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBE0CB4-6079-4D52-8B87-706BE18C11DA}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,6 +727,7 @@
     <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -710,7 +752,9 @@
       <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -739,7 +783,6 @@
       <c r="G2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -748,36 +791,44 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -786,55 +837,78 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
       <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -846,19 +920,211 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0672EC7F-ACA0-48A6-B3F6-A21A4D5B8FC2}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F0A4E3-857E-462A-B4C0-8279C0227926}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -880,120 +1146,31 @@
       <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>